<commit_message>
changes 13 may 2020
</commit_message>
<xml_diff>
--- a/Global Alignment.xlsx
+++ b/Global Alignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\cracking the coding interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\cracking_the_coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5462D7D-049B-45FB-B0EE-72DA15F61DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30BCB39-AEDC-4A85-B754-6533D42B6A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E5F1B2E-67DA-4C8B-8A57-025081495175}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>P</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>Dynamic Programming Approach:</t>
+  </si>
+  <si>
+    <t>L, 1</t>
+  </si>
+  <si>
+    <t>L,2</t>
+  </si>
+  <si>
+    <t>U, 1</t>
+  </si>
+  <si>
+    <t>D, 1</t>
+  </si>
+  <si>
+    <t>D, 2</t>
+  </si>
+  <si>
+    <t>U, 2</t>
+  </si>
+  <si>
+    <t>U, 3</t>
+  </si>
+  <si>
+    <t>D, 0</t>
   </si>
 </sst>
 </file>
@@ -105,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -244,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -260,18 +290,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -281,6 +305,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,50 +630,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6068A7AA-27CD-4C79-9885-DC4AB67B8EE5}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="21"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -656,10 +689,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -675,10 +708,10 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="14"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -688,92 +721,92 @@
         <v>1</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>2</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <v>3</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>4</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="17">
-        <v>0</v>
-      </c>
-      <c r="F8" s="17">
-        <v>1</v>
-      </c>
-      <c r="G8" s="17">
-        <v>2</v>
-      </c>
-      <c r="H8" s="17">
+      <c r="E8" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="16">
         <v>3</v>
       </c>
       <c r="I8" s="3"/>
@@ -783,22 +816,22 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="17">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17">
-        <v>1</v>
-      </c>
-      <c r="G9" s="17">
-        <v>2</v>
-      </c>
-      <c r="H9" s="17">
+      <c r="E9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="16">
         <v>2</v>
       </c>
       <c r="I9" s="3"/>
@@ -808,22 +841,22 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>3</v>
       </c>
-      <c r="E10" s="17">
-        <v>2</v>
-      </c>
-      <c r="F10" s="17">
-        <v>1</v>
-      </c>
-      <c r="G10" s="17">
-        <v>2</v>
-      </c>
-      <c r="H10" s="17">
+      <c r="E10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="16">
         <v>3</v>
       </c>
       <c r="I10" s="3"/>
@@ -833,22 +866,22 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>4</v>
       </c>
-      <c r="E11" s="17">
-        <v>3</v>
-      </c>
-      <c r="F11" s="17">
-        <v>2</v>
-      </c>
-      <c r="G11" s="17">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="E11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="16">
         <v>2</v>
       </c>
       <c r="I11" s="6"/>

</xml_diff>

<commit_message>
problem_1_5 approach for calculating edit distance.
</commit_message>
<xml_diff>
--- a/Global Alignment.xlsx
+++ b/Global Alignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\cracking_the_coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30BCB39-AEDC-4A85-B754-6533D42B6A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC8D88F-2D61-4086-BABC-5F25FCF52941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E5F1B2E-67DA-4C8B-8A57-025081495175}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>P</t>
   </si>
@@ -69,12 +69,6 @@
     <t>score(i-1, j-1)</t>
   </si>
   <si>
-    <t>Global Alignment</t>
-  </si>
-  <si>
-    <t>Needleman-Wunsch Algorithm</t>
-  </si>
-  <si>
     <t>cell(i-1,j)+gap penalty  
 cell(i,j-1)+gap penalty</t>
   </si>
@@ -114,6 +108,15 @@
   </si>
   <si>
     <t>D, 0</t>
+  </si>
+  <si>
+    <t>Problem 1.5</t>
+  </si>
+  <si>
+    <t>(Needleman-Wunsch Algorithm)</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
   </si>
 </sst>
 </file>
@@ -305,13 +308,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,39 +631,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6068A7AA-27CD-4C79-9885-DC4AB67B8EE5}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="C1" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="19"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -668,14 +671,13 @@
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="22"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -688,13 +690,12 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -707,13 +708,12 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="24" t="s">
+      <c r="I4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -721,18 +721,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="D5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="16"/>
@@ -748,18 +747,15 @@
       <c r="G6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="14" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="J6" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="16" t="s">
@@ -777,18 +773,15 @@
       <c r="G7" s="16">
         <v>3</v>
       </c>
-      <c r="H7" s="16">
-        <v>4</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="J7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="16" t="s">
@@ -797,23 +790,20 @@
       <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>25</v>
+      <c r="E8" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="16">
-        <v>3</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="16" t="s">
@@ -822,23 +812,20 @@
       <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="16">
-        <v>2</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="16" t="s">
@@ -848,22 +835,19 @@
         <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="26" t="s">
         <v>21</v>
       </c>
+      <c r="F10" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="G10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="16">
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="16" t="s">
@@ -873,25 +857,22 @@
         <v>4</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="16">
-        <v>2</v>
-      </c>
+      <c r="G11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>